<commit_message>
add screenshot and audio recording
</commit_message>
<xml_diff>
--- a/data/datasheet2.xlsx
+++ b/data/datasheet2.xlsx
@@ -6,15 +6,63 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>Zahid</t>
+  </si>
+  <si>
+    <t>Satkhira</t>
+  </si>
+  <si>
+    <t>01746484619</t>
+  </si>
   <si>
     <t>Hassan</t>
+  </si>
+  <si>
+    <t>Gazipur</t>
+  </si>
+  <si>
+    <t>01678864115</t>
+  </si>
+  <si>
+    <t>The Passionate Programmer</t>
+  </si>
+  <si>
+    <t>Chad Fowler</t>
+  </si>
+  <si>
+    <t>Software Craftmanship</t>
+  </si>
+  <si>
+    <t>Pete McBreen</t>
+  </si>
+  <si>
+    <t>The Art of Agile Development</t>
+  </si>
+  <si>
+    <t>James Shore</t>
+  </si>
+  <si>
+    <t>Continuous Delivery</t>
+  </si>
+  <si>
+    <t>Jez Humble</t>
   </si>
 </sst>
 </file>
@@ -59,15 +107,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>41.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>